<commit_message>
updated Ne input prep, Dps calculation
</commit_message>
<xml_diff>
--- a/steelhead_Ne_result.xlsx
+++ b/steelhead_Ne_result.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyj55\Desktop\LGC-DGS_2022\Team_project\Analysis\Steelhead analysis\Elwha_genetics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF548B3C-F712-4879-8F28-C1F4D620CDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1CCE05D0-1074-4BC2-B581-6F2306913E28}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>Pre_AD</t>
   </si>
@@ -144,11 +143,17 @@
   <si>
     <t>Infinite</t>
   </si>
+  <si>
+    <t>95% CIs (JackKnife)</t>
+  </si>
+  <si>
+    <t>Pre_SBLR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -209,16 +214,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -529,19 +536,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{202705DF-FA7F-41A3-8F26-6DF391DD3CDF}">
-  <dimension ref="C8:K12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A8:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C15" sqref="C15:L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.88671875" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>0</v>
@@ -568,36 +578,36 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="3:11" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
+    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>286.7</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>181.2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>331.3</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="4">
         <v>685</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>338.2</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="4">
         <v>4513</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="2">
         <v>345.3</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="4">
         <v>49.4</v>
       </c>
     </row>
-    <row r="10" spans="3:11" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>9</v>
       </c>
@@ -626,7 +636,7 @@
         <v>68.2</v>
       </c>
     </row>
-    <row r="11" spans="3:11" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
@@ -655,10 +665,140 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="C16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="7">
+        <v>170</v>
+      </c>
+      <c r="E16" s="6">
+        <v>181.2</v>
+      </c>
+      <c r="F16" s="6">
+        <v>49.9</v>
+      </c>
+      <c r="G16" s="7">
+        <v>670.7</v>
+      </c>
+      <c r="H16" s="7">
+        <v>389</v>
+      </c>
+      <c r="I16" s="7">
+        <v>4513</v>
+      </c>
+      <c r="J16" s="6">
+        <v>347.4</v>
+      </c>
+      <c r="K16" s="7">
+        <v>57</v>
+      </c>
+      <c r="L16" s="7">
+        <v>49.4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>116.1</v>
+      </c>
+      <c r="E17">
+        <v>156.6</v>
+      </c>
+      <c r="F17">
+        <v>37.4</v>
+      </c>
+      <c r="G17">
+        <v>236.9</v>
+      </c>
+      <c r="H17" s="1">
+        <v>162</v>
+      </c>
+      <c r="I17">
+        <v>104.5</v>
+      </c>
+      <c r="J17">
+        <v>288.8</v>
+      </c>
+      <c r="K17">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="L17">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2">
+        <v>281.60000000000002</v>
+      </c>
+      <c r="E18" s="2">
+        <v>211.4</v>
+      </c>
+      <c r="F18" s="2">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="2">
+        <v>427.3</v>
+      </c>
+      <c r="K18" s="4">
+        <v>111.9</v>
+      </c>
+      <c r="L18" s="4">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="I22" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update after Synthesis meeting.
</commit_message>
<xml_diff>
--- a/steelhead_Ne_result.xlsx
+++ b/steelhead_Ne_result.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyj55\Desktop\LGC-DGS_2022\Team_project\Analysis\Steelhead analysis\Elwha_genetics\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A5F4E0-0902-4331-B9AF-EBD15493DEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,22 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>Pre_AD</t>
   </si>
@@ -149,11 +140,14 @@
   <si>
     <t>Pre_SBLR</t>
   </si>
+  <si>
+    <t xml:space="preserve">Infinite </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -225,7 +219,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -536,11 +530,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A8:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:L18"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -708,31 +702,31 @@
         <v>8</v>
       </c>
       <c r="D16" s="7">
-        <v>170</v>
-      </c>
-      <c r="E16" s="6">
-        <v>181.2</v>
+        <v>171.8</v>
+      </c>
+      <c r="E16" s="7">
+        <v>182</v>
       </c>
       <c r="F16" s="6">
-        <v>49.9</v>
+        <v>51.3</v>
       </c>
       <c r="G16" s="7">
-        <v>670.7</v>
+        <v>611.79999999999995</v>
       </c>
       <c r="H16" s="7">
-        <v>389</v>
+        <v>384.7</v>
       </c>
       <c r="I16" s="7">
-        <v>4513</v>
+        <v>16458.7</v>
       </c>
       <c r="J16" s="6">
-        <v>347.4</v>
+        <v>346.6</v>
       </c>
       <c r="K16" s="7">
-        <v>57</v>
+        <v>57.3</v>
       </c>
       <c r="L16" s="7">
-        <v>49.4</v>
+        <v>49.7</v>
       </c>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
@@ -740,28 +734,28 @@
         <v>13</v>
       </c>
       <c r="D17">
-        <v>116.1</v>
+        <v>117.1</v>
       </c>
       <c r="E17">
-        <v>156.6</v>
+        <v>157.5</v>
       </c>
       <c r="F17">
-        <v>37.4</v>
+        <v>38.5</v>
       </c>
       <c r="G17">
-        <v>236.9</v>
+        <v>229.5</v>
       </c>
       <c r="H17" s="1">
-        <v>162</v>
+        <v>161.1</v>
       </c>
       <c r="I17">
-        <v>104.5</v>
+        <v>108.6</v>
       </c>
       <c r="J17">
-        <v>288.8</v>
-      </c>
-      <c r="K17">
-        <v>34.799999999999997</v>
+        <v>287.5</v>
+      </c>
+      <c r="K17" s="1">
+        <v>35</v>
       </c>
       <c r="L17">
         <v>23.7</v>
@@ -770,16 +764,16 @@
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="2"/>
       <c r="D18" s="2">
-        <v>281.60000000000002</v>
+        <v>286.2</v>
       </c>
       <c r="E18" s="2">
-        <v>211.4</v>
+        <v>212.1</v>
       </c>
       <c r="F18" s="2">
-        <v>68.099999999999994</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>12</v>
@@ -788,13 +782,13 @@
         <v>12</v>
       </c>
       <c r="J18" s="2">
-        <v>427.3</v>
+        <v>427.4</v>
       </c>
       <c r="K18" s="4">
-        <v>111.9</v>
+        <v>112.3</v>
       </c>
       <c r="L18" s="4">
-        <v>388</v>
+        <v>402.8</v>
       </c>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.3">
@@ -802,6 +796,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>